<commit_message>
Un LIsted Item Adding New Product Feature Added
</commit_message>
<xml_diff>
--- a/SKU.xlsx
+++ b/SKU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nirzaf\source\repos\BabatyeInventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfazrin\source\repos\BabatyeInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BD8775-E469-4EFC-A925-498B36BE345C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E4C74B-0A76-451C-B640-7510E6910BB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="6">
   <si>
     <t>D184T22BLD02</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>D184T22WHD34</t>
+  </si>
+  <si>
+    <t>D184T22BKD03</t>
+  </si>
+  <si>
+    <t>D184T22APD03</t>
   </si>
 </sst>
 </file>
@@ -401,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A453" workbookViewId="0">
-      <selection activeCell="A476" sqref="A476"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -597,7 +603,7 @@
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -757,7 +763,7 @@
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:1">

</xml_diff>

<commit_message>
UI changes in pop up menu for add new item
</commit_message>
<xml_diff>
--- a/SKU.xlsx
+++ b/SKU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfazrin\source\repos\BabatyeInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E4C74B-0A76-451C-B640-7510E6910BB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693241FF-A528-444C-B502-B64138C7872B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:A476"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -723,7 +723,7 @@
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:1">

</xml_diff>

<commit_message>
Adding New Product Issue Fixed
</commit_message>
<xml_diff>
--- a/SKU.xlsx
+++ b/SKU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nirzaf\gitlab\babatye\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfazrin\source\repos\BabatyeInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E67463-621C-4246-BA9F-78108DA5ADBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41D3E3F-6F87-4B48-A213-418E31E6C097}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="8">
   <si>
     <t>D184T22BLD02</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>D184T22DD121</t>
+  </si>
+  <si>
+    <t>D184T22YLD28</t>
+  </si>
+  <si>
+    <t>D184T21AAAAA</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -607,7 +613,9 @@
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="2"/>
+      <c r="A39" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
@@ -625,7 +633,9 @@
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="2"/>
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">

</xml_diff>

<commit_message>
Added prodcut count issue fixed
</commit_message>
<xml_diff>
--- a/SKU.xlsx
+++ b/SKU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfazrin\source\repos\BabatyeInventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nirzaf\gitlab\babatye\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C5EF08-4FD4-4491-B33C-9FABE74DB6CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1C3C98-972E-42D1-BEEB-A0FF969C34A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>D184T22WHD34</t>
   </si>
   <si>
-    <t>D184T22BKD03</t>
-  </si>
-  <si>
     <t>D184T22DD121</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>D184T21BBBBB</t>
+  </si>
+  <si>
+    <t>D184T22BKD04</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -604,17 +604,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:1">
@@ -634,7 +634,7 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:1">

</xml_diff>